<commit_message>
Forgot to save Map Helper
</commit_message>
<xml_diff>
--- a/mods/tuxemon/maps/Map Helper.xlsx
+++ b/mods/tuxemon/maps/Map Helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Tuxemon\mods\tuxemon\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612848AB-E845-4C9D-9B82-C07D697C80B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4449E528-1DBD-44F9-A7E6-A3065E46BF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPC Creator" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="146">
   <si>
     <t>Dante</t>
   </si>
@@ -290,28 +290,210 @@
     <t>Allows you to leave Paper Town</t>
   </si>
   <si>
-    <t>Opens up Riverboat Stations, Daycare Centre</t>
-  </si>
-  <si>
     <t>Positive Condition</t>
   </si>
   <si>
     <t>Negative Condition</t>
   </si>
   <si>
-    <t>Frolicking Rockitten</t>
-  </si>
-  <si>
     <t>wander</t>
   </si>
   <si>
-    <t>Frolicking Conileaf</t>
-  </si>
-  <si>
     <t>conileaf</t>
   </si>
   <si>
     <t>Cond</t>
+  </si>
+  <si>
+    <t>Opens up Riverboat Stations, Daycare Centre, frolicking mons appear</t>
+  </si>
+  <si>
+    <t>Riverboat Captain</t>
+  </si>
+  <si>
+    <t>frolicking</t>
+  </si>
+  <si>
+    <t>Conileaf</t>
+  </si>
+  <si>
+    <t>riverboatcaptain</t>
+  </si>
+  <si>
+    <t>Home Sign</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Home sweet home!</t>
+  </si>
+  <si>
+    <t>Homemaker</t>
+  </si>
+  <si>
+    <t>homemaker</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>Behav output</t>
+  </si>
+  <si>
+    <t>How are you, NAME? \n
+Quiet and selmn as always, I see.</t>
+  </si>
+  <si>
+    <t>act1</t>
+  </si>
+  <si>
+    <t>behav1</t>
+  </si>
+  <si>
+    <t>Resting in Bed</t>
+  </si>
+  <si>
+    <t>restinbed</t>
+  </si>
+  <si>
+    <t>You awake fully rested!</t>
+  </si>
+  <si>
+    <t>mom1</t>
+  </si>
+  <si>
+    <t>mom</t>
+  </si>
+  <si>
+    <t>mom2</t>
+  </si>
+  <si>
+    <t>mom3</t>
+  </si>
+  <si>
+    <t>mom4</t>
+  </si>
+  <si>
+    <t>mom5</t>
+  </si>
+  <si>
+    <t>mom6</t>
+  </si>
+  <si>
+    <t>Good morning sunshine! Rest here any time you like. \n
+Why am I saying that? You live here!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello dear. I should get on with my inventing. \n
+Can't you occupy yourself? \n
+Back in my day, we could amuse ourselves with anything - a stick, a rock, rubbish we found in bins ... </t>
+  </si>
+  <si>
+    <t>Oh, you found yourself a tuxemon. Congratulations! \n
+Why don't you head over to the next town and explore?</t>
+  </si>
+  <si>
+    <t>Welcome back! Look at you, growing up so fast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You know, Granny Piper next door has opened up her Daycare Centre. \n
+Well, not everyone can be an inventor, I guess. </t>
+  </si>
+  <si>
+    <t>Congratulations! You took down the corporations! \n
+Of course, now lots of people don't have a job ... but you did the right thing. I think.</t>
+  </si>
+  <si>
+    <t>TV Watching</t>
+  </si>
+  <si>
+    <t>tvwatch</t>
+  </si>
+  <si>
+    <t>dialog You watch some TV with your beloved level ${{monster_0_level}} ${{monster_0_name}}.</t>
+  </si>
+  <si>
+    <t>Mom</t>
+  </si>
+  <si>
+    <t>spokenmom</t>
+  </si>
+  <si>
+    <t>Speak to your Mom for the first time</t>
+  </si>
+  <si>
+    <t>you speak to your Mom</t>
+  </si>
+  <si>
+    <t>Her dialogue</t>
+  </si>
+  <si>
+    <t>Defeated Shaft</t>
+  </si>
+  <si>
+    <t>shaftdefeated</t>
+  </si>
+  <si>
+    <t>you defeat the Shaft Boss</t>
+  </si>
+  <si>
+    <t>Changes Mom's dialogue</t>
+  </si>
+  <si>
+    <t>Granny Piper</t>
+  </si>
+  <si>
+    <t>granny</t>
+  </si>
+  <si>
+    <t>Speak to Granny Piper for the first time</t>
+  </si>
+  <si>
+    <t>spokengrannypiper</t>
+  </si>
+  <si>
+    <t>you speak to Granny Piper</t>
+  </si>
+  <si>
+    <t>Changes Granny Piper's dialogue</t>
+  </si>
+  <si>
+    <t>grannypiper1</t>
+  </si>
+  <si>
+    <t>grannypiper</t>
+  </si>
+  <si>
+    <t>Oh hello NAME, I didn't see you there among all this hustle and debris! \n
+I can't wait till the Daycare Centre is installed!</t>
+  </si>
+  <si>
+    <t>You know, the Pipers made our fortune in the daycare business! \n
+I've been retired for ten years and I'm getting bored. I want to get back into it!</t>
+  </si>
+  <si>
+    <t>grannypiper2</t>
+  </si>
+  <si>
+    <t>Shopkeeper</t>
+  </si>
+  <si>
+    <t>shopkeeper</t>
+  </si>
+  <si>
+    <t>instore</t>
+  </si>
+  <si>
+    <t>danteshop</t>
+  </si>
+  <si>
+    <t>danteinstore</t>
+  </si>
+  <si>
+    <t>I'm working, boss, I'm working! \n
+Oh, it's just you. You know, we throw out so much of our stock. \n
+It's such a terrible waste. It all goes into the bins behind the back of the Store.</t>
   </si>
 </sst>
 </file>
@@ -632,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +825,10 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -668,71 +850,71 @@
       <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
-        <v>88</v>
-      </c>
       <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>1</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -756,24 +938,28 @@
         <v>75</v>
       </c>
       <c r="H2" t="str">
+        <f>"Create "&amp;A2</f>
+        <v>Create Dante</v>
+      </c>
+      <c r="I2" t="str">
         <f>"not npc_exists "&amp;C2</f>
         <v>not npc_exists dantestop</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <f>"create_npc "&amp;C2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;D2&amp;","&amp;G2</f>
         <v>create_npc dantestop,15,8,shop_assistant,stand</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" t="str">
-        <f>IF(J2="","",CONCATENATE($Z1,$AB1,$AA1,K2,$AD1,L2,AF1,J2,Z1,$AC1))</f>
+      <c r="N2" t="str">
+        <f>IF(K2="","",CONCATENATE($AA1,$AC1,$AB1,L2,$AE1,M2,AG1,K2,AA1,$AD1))</f>
         <v xml:space="preserve">" "monsters": [
         {
             "name": "Agnite",
@@ -781,17 +967,17 @@
         }
 </v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>2</v>
       </c>
-      <c r="Q2" t="str">
-        <f>IF(N2="","",CONCATENATE($Z1,$AA1,O2,$AD1,P2,$AC1))</f>
+      <c r="R2" t="str">
+        <f>IF(O2="","",CONCATENATE($AA1,$AB1,P2,$AE1,Q2,$AD1))</f>
         <v xml:space="preserve">" 
         {
             "name": "Rockitten",
@@ -799,16 +985,16 @@
         }
 </v>
       </c>
-      <c r="U2" t="str">
-        <f>IF(R2="","",CONCATENATE($Z1,$AA1,S2,$AD1,T2,$AC1))</f>
+      <c r="V2" t="str">
+        <f>IF(S2="","",CONCATENATE($AA1,$AB1,T2,$AE1,U2,$AD1))</f>
         <v/>
       </c>
-      <c r="V2" t="str">
-        <f>IF(K2="","","]")</f>
+      <c r="W2" t="str">
+        <f>IF(L2="","","]")</f>
         <v>]</v>
       </c>
-      <c r="W2" t="str">
-        <f>CONCATENATE(W1,C2,X1,D2,M2,Q2,U2,V2,Y1)</f>
+      <c r="X2" t="str">
+        <f>CONCATENATE(X1,C2,Y1,D2,N2,R2,V2,W2,Z1)</f>
         <v>{
     "slug": "dantestop",
     "sprite_name": "shop_assistant" "monsters": [
@@ -824,13 +1010,16 @@
 ]}</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE(SUBSTITUTE(LOWER(A3)," ",""),LOWER(B3))</f>
-        <v>frolickingrockitten</v>
+        <v>rockittenfrolicking</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -842,27 +1031,34 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H4" si="0">"not npc_exists "&amp;C3</f>
-        <v>not npc_exists frolickingrockitten</v>
+        <f t="shared" ref="H3:H10" si="0">"Create "&amp;A3</f>
+        <v>Create Rockitten</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I4" si="1">"create_npc "&amp;C3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;D3&amp;","&amp;G3</f>
-        <v>create_npc frolickingrockitten,24,2,rockitten,wander</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I10" si="1">"not npc_exists "&amp;C3</f>
+        <v>not npc_exists rockittenfrolicking</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="2">"create_npc "&amp;C3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;D3&amp;","&amp;G3</f>
+        <v>create_npc rockittenfrolicking,24,2,rockitten,wander</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
       </c>
       <c r="C4" t="str">
         <f>CONCATENATE(SUBSTITUTE(LOWER(A4)," ",""),LOWER(B4))</f>
-        <v>frolickingconileaf</v>
+        <v>conileaffrolicking</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>27</v>
@@ -871,19 +1067,239 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>not npc_exists frolickingconileaf</v>
+        <v>Create Conileaf</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="1"/>
-        <v>create_npc frolickingconileaf,27,3,conileaf,wander</v>
-      </c>
-      <c r="L4" s="1"/>
+        <v>not npc_exists conileaffrolicking</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc conileaffrolicking,27,3,conileaf,wander</v>
+      </c>
       <c r="M4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A5)," ",""),LOWER(B5))</f>
+        <v>riverboatcaptainpapertown</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Riverboat Captain</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists riverboatcaptainpapertown</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc riverboatcaptainpapertown,4,16,riverboatcaptain,stand</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A6)," ",""),LOWER(B6))</f>
+        <v>homemakerpapertown</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Homemaker</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists homemakerpapertown</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc homemakerpapertown,11,14,homemaker,wander</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A7)," ",""),LOWER(B7))</f>
+        <v>mompapertown</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Mom</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists mompapertown</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc mompapertown,5,5,homemaker,wander</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A8)," ",""),LOWER(B8))</f>
+        <v>grannypiperpapertown</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Granny Piper</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists grannypiperpapertown</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc grannypiperpapertown,3,6,granny,stand</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A9)," ",""),LOWER(B9))</f>
+        <v>shopkeeperpapertown</v>
+      </c>
+      <c r="D9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Shopkeeper</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists shopkeeperpapertown</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc shopkeeperpapertown,4,8,shopkeeper,stand</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" t="str">
+        <f>CONCATENATE(SUBSTITUTE(LOWER(A10)," ",""),LOWER(B10))</f>
+        <v>danteinstore</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>Create Dante</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>not npc_exists danteinstore</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="2"/>
+        <v>create_npc danteinstore,12,7,shop_assistant,stand</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -892,23 +1308,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB86BEE-659D-40E3-BE2C-991E3BDA8715}">
-  <dimension ref="B1:P3"/>
+  <dimension ref="B1:S13"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="37.85546875" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -919,33 +1336,48 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
       <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="H2" s="1" t="s">
+    <row r="2" spans="2:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -955,23 +1387,354 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" s="1"/>
+      <c r="H3" t="str">
         <f>CONCATENATE(B3,"_",C3,"_",D3)</f>
         <v>spyder_papertown_stopthere</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3" si="0">CONCATENATE($L$1,F3)</f>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I13" si="0">CONCATENATE($O$1,H3)</f>
         <v>translated_dialog spyder_papertown_stopthere</v>
       </c>
-      <c r="H3" t="str">
-        <f>$M$1&amp;$N$1&amp;F3&amp;$P$1&amp;CHAR(10)&amp;$O$1&amp;$N$1&amp;E3&amp;$P$1</f>
+      <c r="K3" t="str">
+        <f>$P$1&amp;$Q$1&amp;H3&amp;$S$1&amp;CHAR(10)&amp;$R$1&amp;$Q$1&amp;F3&amp;$S$1</f>
         <v xml:space="preserve">msgid "spyder_papertown_stopthere" 
 msgstr "Hey! What do you think you're doing?\n"
 "It's not safe to go into the wilds unless you have a tuxemon.\n"
 "Come buy one from our shop."" </v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f>"Talk "&amp;D4</f>
+        <v>Talk homemaker</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE(B4,"_",C4,"_",D4)</f>
+        <v>spyder_papertown_homemaker</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_homemaker</v>
+      </c>
+      <c r="J4" t="str">
+        <f>"talk "&amp;E4</f>
+        <v>talk homemaker</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" ref="G5:G13" si="1">"Talk "&amp;D5</f>
+        <v>Talk mom1</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5:H13" si="2">CONCATENATE(B5,"_",C5,"_",D5)</f>
+        <v>spyder_papertown_mom1</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom1</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"talk "&amp;E5</f>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk mom2</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_mom2</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom2</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ref="J6:J13" si="3">"talk "&amp;E6</f>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk mom3</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_mom3</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom3</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk mom4</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_mom4</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom4</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk mom5</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_mom5</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom5</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk mom6</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_mom6</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_mom6</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>talk mom</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk grannypiper1</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_grannypiper1</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_grannypiper1</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>talk grannypiper</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk grannypiper2</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_grannypiper2</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_grannypiper2</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>talk grannypiper</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Talk danteshop</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>spyder_papertown_danteshop</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>translated_dialog spyder_papertown_danteshop</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>talk danteinstore</v>
       </c>
     </row>
   </sheetData>
@@ -981,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A32D68-480F-4057-AFCF-ADC7DB3A66FB}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,6 +2011,96 @@
 msgstr "Sunnyside Manor: If we are not home leave a message with our housekeeper." </v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" t="str">
+        <f>CONCATENATE(B10,"_",C10,"_",D10)</f>
+        <v>spyder_papertown_home</v>
+      </c>
+      <c r="G10" t="str">
+        <f>CONCATENATE($L$1,F10)</f>
+        <v>translated_dialog spyder_papertown_home</v>
+      </c>
+      <c r="H10" t="str">
+        <f>$M$1&amp;$N$1&amp;F10&amp;$P$1&amp;CHAR(10)&amp;$O$1&amp;$N$1&amp;E10&amp;$P$1</f>
+        <v xml:space="preserve">msgid "spyder_papertown_home" 
+msgstr "Home sweet home!" </v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="str">
+        <f>CONCATENATE(B11,"_",C11,"_",D11)</f>
+        <v>spyder_papertown_restinbed</v>
+      </c>
+      <c r="G11" t="str">
+        <f>CONCATENATE($L$1,F11)</f>
+        <v>translated_dialog spyder_papertown_restinbed</v>
+      </c>
+      <c r="H11" t="str">
+        <f>$M$1&amp;$N$1&amp;F11&amp;$P$1&amp;CHAR(10)&amp;$O$1&amp;$N$1&amp;E11&amp;$P$1</f>
+        <v xml:space="preserve">msgid "spyder_papertown_restinbed" 
+msgstr "You awake fully rested!" </v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" t="str">
+        <f>CONCATENATE(B12,"_",C12,"_",D12)</f>
+        <v>spyder_papertown_tvwatch</v>
+      </c>
+      <c r="G12" t="str">
+        <f>CONCATENATE($L$1,F12)</f>
+        <v>translated_dialog spyder_papertown_tvwatch</v>
+      </c>
+      <c r="H12" t="str">
+        <f>$M$1&amp;$N$1&amp;F12&amp;$P$1&amp;CHAR(10)&amp;$O$1&amp;$N$1&amp;E12&amp;$P$1</f>
+        <v xml:space="preserve">msgid "spyder_papertown_tvwatch" 
+msgstr "dialog You watch some TV with your beloved level ${{monster_0_level}} ${{monster_0_name}}." </v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1255,17 +2108,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F09B0BC-4413-48EC-AF81-1BA624AD7E0E}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1286,10 +2140,10 @@
         <v>79</v>
       </c>
       <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>82</v>
-      </c>
-      <c r="G1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,10 +2153,6 @@
       <c r="E2" t="s">
         <v>80</v>
       </c>
-      <c r="F2" t="str">
-        <f>"is variable_set "&amp;B2&amp;":yes"</f>
-        <v>is variable_set :yes</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1318,7 +2168,7 @@
         <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F3" t="str">
         <f>"is variable_set "&amp;B3&amp;":yes"</f>
@@ -1327,6 +2177,81 @@
       <c r="G3" t="str">
         <f>"not variable_set "&amp;B3&amp;":yes"</f>
         <v>not variable_set timberreached:yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"is variable_set "&amp;B4&amp;":yes"</f>
+        <v>is variable_set spokenmom:yes</v>
+      </c>
+      <c r="G4" t="str">
+        <f>"not variable_set "&amp;B4&amp;":yes"</f>
+        <v>not variable_set spokenmom:yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"is variable_set "&amp;B5&amp;":yes"</f>
+        <v>is variable_set shaftdefeated:yes</v>
+      </c>
+      <c r="G5" t="str">
+        <f>"not variable_set "&amp;B5&amp;":yes"</f>
+        <v>not variable_set shaftdefeated:yes</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" t="str">
+        <f>"is variable_set "&amp;B6&amp;":yes"</f>
+        <v>is variable_set spokengrannypiper:yes</v>
+      </c>
+      <c r="G6" t="str">
+        <f>"not variable_set "&amp;B6&amp;":yes"</f>
+        <v>not variable_set spokengrannypiper:yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing a few bugs
</commit_message>
<xml_diff>
--- a/mods/tuxemon/maps/Map Helper.xlsx
+++ b/mods/tuxemon/maps/Map Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\tuxemon-development-win64\exe.win-amd64-3.8\mods\tuxemon\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9121FBF-6E66-43BC-A783-4B404E75CAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6595A805-D31B-4642-B00E-46CC531F4144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="1411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1413">
   <si>
     <t>Dante</t>
   </si>
@@ -4276,6 +4276,12 @@
   </si>
   <si>
     <t>Why yes, I am the inventor of the Extreme Restraints. \n What are they, I hear you ask? \n Only a set of manacles so powerful that even a dragon could not escape them. \n They are being used in the containment unit to make sure none of the infected tuxemon escape.</t>
+  </si>
+  <si>
+    <t>snugglepot2</t>
+  </si>
+  <si>
+    <t>Wow! One day I'm going to be a trainer just like you!</t>
   </si>
 </sst>
 </file>
@@ -16262,7 +16268,7 @@
   <dimension ref="A1:AG13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16453,10 +16459,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB86BEE-659D-40E3-BE2C-991E3BDA8715}">
-  <dimension ref="A1:R375"/>
+  <dimension ref="A1:R376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E346" sqref="E346"/>
+    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J375" sqref="J375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22136,7 +22142,7 @@
         <v>740</v>
       </c>
       <c r="F168" s="1" t="str">
-        <f t="shared" ref="F168:F375" si="40">"Talk "&amp;C168</f>
+        <f t="shared" ref="F168:F376" si="40">"Talk "&amp;C168</f>
         <v>Talk scientist</v>
       </c>
       <c r="G168" t="str">
@@ -28001,7 +28007,7 @@
         <v>translated_dialog spyder_mansion_drinkingbuddyb1</v>
       </c>
       <c r="J357" t="str">
-        <f t="shared" ref="J357:J375" si="78">$O$1&amp;$P$1&amp;G357&amp;$R$1&amp;CHAR(10)&amp;$Q$1&amp;$P$1&amp;E357&amp;$R$1</f>
+        <f t="shared" ref="J357:J376" si="78">$O$1&amp;$P$1&amp;G357&amp;$R$1&amp;CHAR(10)&amp;$Q$1&amp;$P$1&amp;E357&amp;$R$1</f>
         <v xml:space="preserve">msgid "spyder_mansion_drinkingbuddyb1" 
 msgstr "We started singing an old sea shanty, and by the time we'd done the Captain was missing!" </v>
       </c>
@@ -28179,11 +28185,11 @@
         <v>Talk aquemini1</v>
       </c>
       <c r="G363" t="str">
-        <f t="shared" ref="G363:G375" si="79">CONCATENATE(A363,"_",B363,"_",C363)</f>
+        <f t="shared" ref="G363:G376" si="79">CONCATENATE(A363,"_",B363,"_",C363)</f>
         <v>spyder_dryadsgrove_aquemini1</v>
       </c>
       <c r="H363" t="str">
-        <f t="shared" ref="H363:H375" si="80">CONCATENATE($N$1,G363)</f>
+        <f t="shared" ref="H363:H376" si="80">CONCATENATE($N$1,G363)</f>
         <v>translated_dialog spyder_dryadsgrove_aquemini1</v>
       </c>
       <c r="J363" t="str">
@@ -28562,6 +28568,37 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">msgid "spyder_successful_boulder" 
 msgstr "The sledgehammer smashes the boulder apart." </v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>4</v>
+      </c>
+      <c r="B376" t="s">
+        <v>724</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E376" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F376" s="1" t="str">
+        <f t="shared" si="40"/>
+        <v>Talk snugglepot2</v>
+      </c>
+      <c r="G376" t="str">
+        <f t="shared" si="79"/>
+        <v>spyder_leatherhouse2_snugglepot2</v>
+      </c>
+      <c r="H376" t="str">
+        <f t="shared" si="80"/>
+        <v>translated_dialog spyder_leatherhouse2_snugglepot2</v>
+      </c>
+      <c r="J376" t="str">
+        <f t="shared" si="78"/>
+        <v xml:space="preserve">msgid "spyder_leatherhouse2_snugglepot2" 
+msgstr "Wow! One day I'm going to be a trainer just like you!" </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated maps from play through
Changes to maps and dialogue from another playthrough
</commit_message>
<xml_diff>
--- a/mods/tuxemon/maps/Map Helper.xlsx
+++ b/mods/tuxemon/maps/Map Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\tuxemon-development-win64\exe.win-amd64-3.8\mods\tuxemon\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6595A805-D31B-4642-B00E-46CC531F4144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B3CCF4-85C6-4016-A9DC-ED0E73A7B168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3396,9 +3396,6 @@
     <t xml:space="preserve">He's so hard on himself, never happy with something he's painted. He's so forgetful, too. Perhaps I could buy a painting </t>
   </si>
   <si>
-    <t>A newspaper clipping is on the wall. It begins: \n "The famous art critic has put away his poison pen and picked up the paint brush. After years of tearing down artists, can he do any better himself?"</t>
-  </si>
-  <si>
     <t>Magnificent! I didn't know I had it in me. \n I don't know what those artist were complaining about - painting is easy!</t>
   </si>
   <si>
@@ -4282,6 +4279,9 @@
   </si>
   <si>
     <t>Wow! One day I'm going to be a trainer just like you!</t>
+  </si>
+  <si>
+    <t>A newspaper clipping is on the wall. It begins: \n "The famous art critic has put away his poison pen and picked up the paint brush. \n After years of tearing down artists, can he do any better himself?"</t>
   </si>
 </sst>
 </file>
@@ -14157,26 +14157,26 @@
     </row>
     <row r="118" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B118" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" t="s">
         <v>1126</v>
-      </c>
-      <c r="B118" t="s">
-        <v>4</v>
-      </c>
-      <c r="C118" t="s">
-        <v>1127</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="54"/>
         <v>spyder_searoutec_nigel</v>
       </c>
       <c r="E118" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="I118" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="J118" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="K118">
         <v>36</v>
@@ -14218,26 +14218,26 @@
     </row>
     <row r="119" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" ref="D119:D127" si="56">CONCATENATE(B119,"_",LOWER(C119),IF(C119="","","_"),SUBSTITUTE(LOWER(A119)," ",""))</f>
         <v>spyder_searoutec_river</v>
       </c>
       <c r="E119" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="I119" t="s">
+        <v>1140</v>
+      </c>
+      <c r="J119" t="s">
         <v>1141</v>
-      </c>
-      <c r="J119" t="s">
-        <v>1142</v>
       </c>
       <c r="K119">
         <v>24</v>
@@ -14279,20 +14279,20 @@
     </row>
     <row r="120" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B120" t="s">
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="56"/>
         <v>spyder_searoutec_wade</v>
       </c>
       <c r="E120" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="I120" t="s">
         <v>616</v>
@@ -14368,20 +14368,20 @@
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B121" t="s">
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="56"/>
         <v>spyder_searoutec_gil</v>
       </c>
       <c r="E121" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="I121" t="s">
         <v>506</v>
@@ -14402,10 +14402,10 @@
         <v>22</v>
       </c>
       <c r="O121" t="s">
+        <v>1142</v>
+      </c>
+      <c r="P121" t="s">
         <v>1143</v>
-      </c>
-      <c r="P121" t="s">
-        <v>1144</v>
       </c>
       <c r="Q121">
         <v>24</v>
@@ -14457,26 +14457,26 @@
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B122" t="s">
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="56"/>
         <v>spyder_searoutec_leek</v>
       </c>
       <c r="E122" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="I122" t="s">
+        <v>1144</v>
+      </c>
+      <c r="J122" t="s">
         <v>1145</v>
-      </c>
-      <c r="J122" t="s">
-        <v>1146</v>
       </c>
       <c r="K122">
         <v>27</v>
@@ -14518,26 +14518,26 @@
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B123" t="s">
         <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="56"/>
         <v>spyder_searoutec_beech</v>
       </c>
       <c r="E123" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="I123" t="s">
+        <v>1146</v>
+      </c>
+      <c r="J123" t="s">
         <v>1147</v>
-      </c>
-      <c r="J123" t="s">
-        <v>1148</v>
       </c>
       <c r="K123">
         <v>26</v>
@@ -14579,13 +14579,13 @@
     </row>
     <row r="124" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B124" t="s">
         <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D124" t="str">
         <f t="shared" si="56"/>
@@ -14595,10 +14595,10 @@
         <v>481</v>
       </c>
       <c r="I124" t="s">
+        <v>1148</v>
+      </c>
+      <c r="J124" t="s">
         <v>1149</v>
-      </c>
-      <c r="J124" t="s">
-        <v>1150</v>
       </c>
       <c r="K124">
         <v>26</v>
@@ -14640,13 +14640,13 @@
     </row>
     <row r="125" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D125" t="str">
         <f t="shared" si="56"/>
@@ -14656,10 +14656,10 @@
         <v>580</v>
       </c>
       <c r="I125" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J125" t="s">
         <v>1151</v>
-      </c>
-      <c r="J125" t="s">
-        <v>1152</v>
       </c>
       <c r="K125">
         <v>24</v>
@@ -14701,13 +14701,13 @@
     </row>
     <row r="126" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B126" t="s">
         <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D126" t="str">
         <f t="shared" si="56"/>
@@ -14735,10 +14735,10 @@
         <v>22</v>
       </c>
       <c r="O126" t="s">
+        <v>1152</v>
+      </c>
+      <c r="P126" t="s">
         <v>1153</v>
-      </c>
-      <c r="P126" t="s">
-        <v>1154</v>
       </c>
       <c r="Q126">
         <v>22</v>
@@ -14790,20 +14790,20 @@
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B127" t="s">
         <v>4</v>
       </c>
       <c r="C127" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D127" t="str">
         <f t="shared" si="56"/>
         <v>spyder_dragonscave_tomas</v>
       </c>
       <c r="E127" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S127" s="9" t="str">
         <f t="shared" si="50"/>
@@ -14837,20 +14837,20 @@
     </row>
     <row r="128" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B128" t="s">
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D128" t="str">
         <f t="shared" ref="D128:D168" si="57">CONCATENATE(B128,"_",LOWER(C128),IF(C128="","","_"),SUBSTITUTE(LOWER(A128)," ",""))</f>
         <v>spyder_dragonscave_lessa</v>
       </c>
       <c r="E128" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S128" s="9" t="str">
         <f t="shared" si="50"/>
@@ -14884,20 +14884,20 @@
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
       </c>
       <c r="C129" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D129" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dragonscave_cailin</v>
       </c>
       <c r="E129" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S129" s="9" t="str">
         <f t="shared" si="50"/>
@@ -14931,20 +14931,20 @@
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B130" t="s">
         <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dragonscave_griffin</v>
       </c>
       <c r="E130" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S130" s="9" t="str">
         <f t="shared" si="50"/>
@@ -14978,20 +14978,20 @@
     </row>
     <row r="131" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B131" t="s">
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D131" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dragonscave_daenny</v>
       </c>
       <c r="E131" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S131" s="9" t="str">
         <f t="shared" si="50"/>
@@ -15025,20 +15025,20 @@
     </row>
     <row r="132" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B132" t="s">
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D132" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dragonscave_benden</v>
       </c>
       <c r="E132" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S132" s="9" t="str">
         <f t="shared" si="50"/>
@@ -15072,20 +15072,20 @@
     </row>
     <row r="133" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B133" t="s">
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D133" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dragonscave_mal</v>
       </c>
       <c r="E133" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="S133" s="9" t="str">
         <f t="shared" si="50"/>
@@ -15119,13 +15119,13 @@
     </row>
     <row r="134" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B134" t="s">
         <v>4</v>
       </c>
       <c r="C134" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D134" t="str">
         <f t="shared" si="57"/>
@@ -15166,13 +15166,13 @@
     </row>
     <row r="135" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B135" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s">
         <v>1198</v>
-      </c>
-      <c r="B135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C135" t="s">
-        <v>1199</v>
       </c>
       <c r="D135" t="str">
         <f t="shared" si="57"/>
@@ -15219,7 +15219,7 @@
         <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D136" t="str">
         <f t="shared" si="57"/>
@@ -15260,7 +15260,7 @@
     </row>
     <row r="137" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B137" t="s">
         <v>4</v>
@@ -15273,7 +15273,7 @@
         <v>spyder_flower_cady</v>
       </c>
       <c r="E137" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="S137" s="9" t="str">
         <f t="shared" si="50"/>
@@ -15307,7 +15307,7 @@
     </row>
     <row r="138" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B138" t="s">
         <v>4</v>
@@ -15354,7 +15354,7 @@
     </row>
     <row r="139" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B139" t="s">
         <v>4</v>
@@ -15367,7 +15367,7 @@
         <v>spyder_flower_sandy</v>
       </c>
       <c r="E139" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="S139" s="9" t="str">
         <f t="shared" si="50"/>
@@ -15401,7 +15401,7 @@
     </row>
     <row r="140" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B140" t="s">
         <v>4</v>
@@ -15444,7 +15444,7 @@
     </row>
     <row r="141" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B141" t="s">
         <v>4</v>
@@ -15479,7 +15479,7 @@
     </row>
     <row r="142" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B142" t="s">
         <v>4</v>
@@ -15514,7 +15514,7 @@
     </row>
     <row r="143" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B143" t="s">
         <v>4</v>
@@ -15549,7 +15549,7 @@
     </row>
     <row r="144" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B144" t="s">
         <v>4</v>
@@ -15562,7 +15562,7 @@
         <v>spyder_omnichannel_strauss</v>
       </c>
       <c r="E144" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="W144" t="str">
         <f t="shared" si="55"/>
@@ -15584,7 +15584,7 @@
     </row>
     <row r="145" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B145" t="s">
         <v>4</v>
@@ -15597,7 +15597,7 @@
         <v>spyder_omnichannel_beaverbrook</v>
       </c>
       <c r="E145" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="W145" t="str">
         <f t="shared" si="55"/>
@@ -15619,7 +15619,7 @@
     </row>
     <row r="146" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B146" t="s">
         <v>4</v>
@@ -15632,7 +15632,7 @@
         <v>spyder_omnichannel_worm</v>
       </c>
       <c r="E146" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="W146" t="str">
         <f t="shared" si="55"/>
@@ -15654,7 +15654,7 @@
     </row>
     <row r="147" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B147" t="s">
         <v>4</v>
@@ -15667,7 +15667,7 @@
         <v>spyder_omnichannel_thedukeofdeadair</v>
       </c>
       <c r="E147" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="W147" t="str">
         <f t="shared" si="55"/>
@@ -15689,13 +15689,13 @@
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="B148" t="s">
         <v>4</v>
       </c>
       <c r="C148" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="57"/>
@@ -15724,13 +15724,13 @@
     </row>
     <row r="149" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B149" t="s">
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="57"/>
@@ -15759,13 +15759,13 @@
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="B150" t="s">
         <v>4</v>
       </c>
       <c r="C150" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="57"/>
@@ -15800,7 +15800,7 @@
         <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="57"/>
@@ -15829,13 +15829,13 @@
     </row>
     <row r="152" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B152" t="s">
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="57"/>
@@ -15874,7 +15874,7 @@
         <v>spyder_riverboatcaptain</v>
       </c>
       <c r="E153" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="W153" t="str">
         <f t="shared" si="55"/>
@@ -15896,20 +15896,20 @@
     </row>
     <row r="154" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" t="s">
         <v>1317</v>
-      </c>
-      <c r="B154" t="s">
-        <v>4</v>
-      </c>
-      <c r="C154" t="s">
-        <v>1318</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="57"/>
         <v>spyder_mansion_drinkingbuddya</v>
       </c>
       <c r="E154" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="W154" t="str">
         <f t="shared" si="55"/>
@@ -15931,13 +15931,13 @@
     </row>
     <row r="155" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B155" t="s">
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="57"/>
@@ -15966,20 +15966,20 @@
     </row>
     <row r="156" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B156" t="s">
         <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D156" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_aquemini</v>
       </c>
       <c r="E156" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="W156" t="str">
         <f t="shared" si="55"/>
@@ -15993,20 +15993,20 @@
     </row>
     <row r="157" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B157" t="s">
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D157" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_ignatia</v>
       </c>
       <c r="E157" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="W157" t="str">
         <f t="shared" si="55"/>
@@ -16020,20 +16020,20 @@
     </row>
     <row r="158" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B158" t="s">
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_petra</v>
       </c>
       <c r="E158" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="W158" t="str">
         <f t="shared" si="55"/>
@@ -16047,20 +16047,20 @@
     </row>
     <row r="159" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B159" t="s">
         <v>4</v>
       </c>
       <c r="C159" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D159" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_ferris</v>
       </c>
       <c r="E159" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="W159" t="str">
         <f t="shared" si="55"/>
@@ -16074,20 +16074,20 @@
     </row>
     <row r="160" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B160" t="s">
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_sylvia</v>
       </c>
       <c r="E160" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="W160" t="str">
         <f t="shared" si="55"/>
@@ -16101,20 +16101,20 @@
     </row>
     <row r="161" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B161" t="s">
         <v>4</v>
       </c>
       <c r="C161" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="57"/>
         <v>spyder_dryadsgrove_volcoli</v>
       </c>
       <c r="E161" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="W161" t="str">
         <f t="shared" si="55"/>
@@ -16146,7 +16146,7 @@
     </row>
     <row r="163" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="57"/>
@@ -16200,7 +16200,7 @@
     </row>
     <row r="166" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="57"/>
@@ -16218,7 +16218,7 @@
     </row>
     <row r="167" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="57"/>
@@ -16236,7 +16236,7 @@
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="57"/>
@@ -16311,10 +16311,10 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B3" t="s">
         <v>1378</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1379</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE($D$1,$E$1,B3,$G$1,CHAR(10),$F$1,$E$1,A3,$G$1)</f>
@@ -16324,10 +16324,10 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C13" si="0">CONCATENATE($D$1,$E$1,B4,$G$1,CHAR(10),$F$1,$E$1,A4,$G$1)</f>
@@ -16337,10 +16337,10 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B5" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -16350,10 +16350,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B6" t="s">
         <v>1384</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1385</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -16363,10 +16363,10 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B7" t="s">
         <v>1388</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1389</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -16376,10 +16376,10 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B8" t="s">
         <v>1390</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1391</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -16389,7 +16389,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B9" t="s">
         <v>912</v>
@@ -16415,10 +16415,10 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B11" t="s">
         <v>1399</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1400</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -16428,10 +16428,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B12" t="s">
         <v>1401</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1402</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -16441,7 +16441,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B13" t="s">
         <v>268</v>
@@ -16461,8 +16461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB86BEE-659D-40E3-BE2C-991E3BDA8715}">
   <dimension ref="A1:R376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J375" sqref="J375"/>
+    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E286" sqref="E286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19187,7 +19187,7 @@
         <v>461</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="F75" s="1" t="str">
         <f t="shared" si="22"/>
@@ -19218,7 +19218,7 @@
         <v>462</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="F76" s="1" t="str">
         <f t="shared" si="22"/>
@@ -19745,7 +19745,7 @@
         <v>524</v>
       </c>
       <c r="E93" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="F93" s="1" t="str">
         <f t="shared" si="22"/>
@@ -19931,7 +19931,7 @@
         <v>545</v>
       </c>
       <c r="E99" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F99" s="1" t="str">
         <f t="shared" si="22"/>
@@ -20899,7 +20899,7 @@
         <v>646</v>
       </c>
       <c r="E128" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="F128" s="1" t="str">
         <f t="shared" si="22"/>
@@ -20961,7 +20961,7 @@
         <v>648</v>
       </c>
       <c r="E130" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="F130" s="1" t="str">
         <f t="shared" si="22"/>
@@ -21454,7 +21454,7 @@
         <v>664</v>
       </c>
       <c r="C146" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="E146" t="s">
         <v>751</v>
@@ -21516,7 +21516,7 @@
         <v>664</v>
       </c>
       <c r="C148" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="E148" t="s">
         <v>754</v>
@@ -24061,7 +24061,7 @@
         <v>943</v>
       </c>
       <c r="E230" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="F230" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25670,7 +25670,7 @@
         <v>664</v>
       </c>
       <c r="C282" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E282" t="s">
         <v>1114</v>
@@ -25701,7 +25701,7 @@
         <v>664</v>
       </c>
       <c r="C283" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E283" t="s">
         <v>1116</v>
@@ -25732,7 +25732,7 @@
         <v>664</v>
       </c>
       <c r="C284" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E284" t="s">
         <v>1115</v>
@@ -25763,10 +25763,10 @@
         <v>664</v>
       </c>
       <c r="C285" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E285" t="s">
-        <v>1117</v>
+        <v>1412</v>
       </c>
       <c r="F285" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25783,7 +25783,7 @@
       <c r="J285" t="str">
         <f t="shared" si="52"/>
         <v xml:space="preserve">msgid "spyder_flower_artist_clipping" 
-msgstr "A newspaper clipping is on the wall. It begins: \n "The famous art critic has put away his poison pen and picked up the paint brush. After years of tearing down artists, can he do any better himself?"" </v>
+msgstr "A newspaper clipping is on the wall. It begins: \n "The famous art critic has put away his poison pen and picked up the paint brush. \n After years of tearing down artists, can he do any better himself?"" </v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.3">
@@ -25794,10 +25794,10 @@
         <v>664</v>
       </c>
       <c r="C286" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E286" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F286" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25825,10 +25825,10 @@
         <v>664</v>
       </c>
       <c r="C287" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E287" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F287" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25853,13 +25853,13 @@
         <v>4</v>
       </c>
       <c r="B288" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C288" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E288" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F288" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25884,13 +25884,13 @@
         <v>4</v>
       </c>
       <c r="B289" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C289" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E289" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="F289" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25915,13 +25915,13 @@
         <v>4</v>
       </c>
       <c r="B290" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C290" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E290" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F290" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25946,13 +25946,13 @@
         <v>4</v>
       </c>
       <c r="B291" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C291" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E291" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F291" s="1" t="str">
         <f t="shared" si="40"/>
@@ -25977,13 +25977,13 @@
         <v>4</v>
       </c>
       <c r="B292" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C292" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E292" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F292" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26008,13 +26008,13 @@
         <v>4</v>
       </c>
       <c r="B293" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C293" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E293" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="F293" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26039,13 +26039,13 @@
         <v>4</v>
       </c>
       <c r="B294" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C294" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E294" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F294" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26070,13 +26070,13 @@
         <v>4</v>
       </c>
       <c r="B295" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C295" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="E295" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F295" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26101,13 +26101,13 @@
         <v>4</v>
       </c>
       <c r="B296" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C296" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="E296" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="F296" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26132,13 +26132,13 @@
         <v>4</v>
       </c>
       <c r="B297" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C297" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E297" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="F297" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26163,13 +26163,13 @@
         <v>4</v>
       </c>
       <c r="B298" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C298" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E298" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="F298" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26194,13 +26194,13 @@
         <v>4</v>
       </c>
       <c r="B299" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C299" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="E299" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="F299" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26225,13 +26225,13 @@
         <v>4</v>
       </c>
       <c r="B300" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C300" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E300" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="F300" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26256,13 +26256,13 @@
         <v>4</v>
       </c>
       <c r="B301" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C301" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E301" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="F301" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26287,13 +26287,13 @@
         <v>4</v>
       </c>
       <c r="B302" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C302" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E302" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F302" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26318,13 +26318,13 @@
         <v>4</v>
       </c>
       <c r="B303" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C303" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="E303" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="F303" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26349,13 +26349,13 @@
         <v>4</v>
       </c>
       <c r="B304" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C304" t="s">
         <v>744</v>
       </c>
       <c r="E304" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F304" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26380,13 +26380,13 @@
         <v>4</v>
       </c>
       <c r="B305" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C305" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E305" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="F305" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26411,13 +26411,13 @@
         <v>4</v>
       </c>
       <c r="B306" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C306" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="E306" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F306" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26442,13 +26442,13 @@
         <v>4</v>
       </c>
       <c r="B307" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C307" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="E307" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F307" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26473,13 +26473,13 @@
         <v>4</v>
       </c>
       <c r="B308" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C308" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="E308" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="F308" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26504,13 +26504,13 @@
         <v>4</v>
       </c>
       <c r="B309" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C309" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="E309" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="F309" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26538,10 +26538,10 @@
         <v>200</v>
       </c>
       <c r="C310" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E310" t="s">
         <v>1227</v>
-      </c>
-      <c r="E310" t="s">
-        <v>1228</v>
       </c>
       <c r="F310" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26569,10 +26569,10 @@
         <v>200</v>
       </c>
       <c r="C311" t="s">
+        <v>1228</v>
+      </c>
+      <c r="E311" t="s">
         <v>1229</v>
-      </c>
-      <c r="E311" t="s">
-        <v>1230</v>
       </c>
       <c r="F311" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26600,10 +26600,10 @@
         <v>200</v>
       </c>
       <c r="C312" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E312" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="F312" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26631,10 +26631,10 @@
         <v>200</v>
       </c>
       <c r="C313" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="E313" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="F313" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26662,10 +26662,10 @@
         <v>200</v>
       </c>
       <c r="C314" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="E314" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F314" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26693,10 +26693,10 @@
         <v>200</v>
       </c>
       <c r="C315" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="E315" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="F315" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26724,10 +26724,10 @@
         <v>200</v>
       </c>
       <c r="C316" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="E316" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="F316" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26755,10 +26755,10 @@
         <v>200</v>
       </c>
       <c r="C317" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="E317" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="F317" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26789,7 +26789,7 @@
         <v>541</v>
       </c>
       <c r="E318" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="F318" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26817,10 +26817,10 @@
         <v>200</v>
       </c>
       <c r="C319" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E319" t="s">
         <v>1247</v>
-      </c>
-      <c r="E319" t="s">
-        <v>1248</v>
       </c>
       <c r="F319" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26848,10 +26848,10 @@
         <v>200</v>
       </c>
       <c r="C320" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E320" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="F320" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26879,10 +26879,10 @@
         <v>200</v>
       </c>
       <c r="C321" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E321" t="s">
         <v>1251</v>
-      </c>
-      <c r="E321" t="s">
-        <v>1252</v>
       </c>
       <c r="F321" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26907,13 +26907,13 @@
         <v>4</v>
       </c>
       <c r="B322" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C322" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="E322" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="F322" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26938,13 +26938,13 @@
         <v>4</v>
       </c>
       <c r="B323" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C323" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E323" t="s">
         <v>1256</v>
-      </c>
-      <c r="E323" t="s">
-        <v>1257</v>
       </c>
       <c r="F323" s="1" t="str">
         <f t="shared" si="40"/>
@@ -26969,13 +26969,13 @@
         <v>4</v>
       </c>
       <c r="B324" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C324" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E324" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F324" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27000,13 +27000,13 @@
         <v>4</v>
       </c>
       <c r="B325" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C325" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="E325" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="F325" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27031,13 +27031,13 @@
         <v>4</v>
       </c>
       <c r="B326" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C326" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="E326" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="F326" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27062,13 +27062,13 @@
         <v>4</v>
       </c>
       <c r="B327" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C327" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E327" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="F327" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27093,13 +27093,13 @@
         <v>4</v>
       </c>
       <c r="B328" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C328" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E328" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="F328" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27124,13 +27124,13 @@
         <v>4</v>
       </c>
       <c r="B329" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C329" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E329" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="F329" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27155,13 +27155,13 @@
         <v>4</v>
       </c>
       <c r="B330" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C330" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="E330" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="F330" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27186,13 +27186,13 @@
         <v>4</v>
       </c>
       <c r="B331" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C331" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E331" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="F331" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27217,13 +27217,13 @@
         <v>4</v>
       </c>
       <c r="B332" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C332" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E332" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="F332" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27248,13 +27248,13 @@
         <v>4</v>
       </c>
       <c r="B333" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C333" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E333" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="F333" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27279,13 +27279,13 @@
         <v>4</v>
       </c>
       <c r="B334" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C334" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E334" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="F334" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27310,13 +27310,13 @@
         <v>4</v>
       </c>
       <c r="B335" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C335" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E335" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F335" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27341,13 +27341,13 @@
         <v>4</v>
       </c>
       <c r="B336" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C336" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E336" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="F336" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27372,13 +27372,13 @@
         <v>4</v>
       </c>
       <c r="B337" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C337" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E337" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="F337" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27403,13 +27403,13 @@
         <v>4</v>
       </c>
       <c r="B338" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C338" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E338" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="F338" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27434,13 +27434,13 @@
         <v>4</v>
       </c>
       <c r="B339" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C339" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E339" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="F339" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27465,13 +27465,13 @@
         <v>4</v>
       </c>
       <c r="B340" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C340" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E340" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="F340" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27496,13 +27496,13 @@
         <v>4</v>
       </c>
       <c r="B341" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C341" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E341" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="F341" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27527,13 +27527,13 @@
         <v>4</v>
       </c>
       <c r="B342" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C342" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E342" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F342" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27558,13 +27558,13 @@
         <v>4</v>
       </c>
       <c r="B343" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C343" t="s">
         <v>800</v>
       </c>
       <c r="E343" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F343" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27589,13 +27589,13 @@
         <v>4</v>
       </c>
       <c r="B344" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C344" t="s">
         <v>801</v>
       </c>
       <c r="E344" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F344" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27620,13 +27620,13 @@
         <v>4</v>
       </c>
       <c r="B345" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C345" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E345" t="s">
         <v>1289</v>
-      </c>
-      <c r="E345" t="s">
-        <v>1290</v>
       </c>
       <c r="F345" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27707,13 +27707,13 @@
         <v>4</v>
       </c>
       <c r="B348" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C348" t="s">
         <v>1300</v>
       </c>
-      <c r="C348" t="s">
+      <c r="E348" t="s">
         <v>1301</v>
-      </c>
-      <c r="E348" t="s">
-        <v>1302</v>
       </c>
       <c r="F348" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27738,13 +27738,13 @@
         <v>4</v>
       </c>
       <c r="B349" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C349" t="s">
         <v>545</v>
       </c>
       <c r="E349" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F349" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27769,13 +27769,13 @@
         <v>4</v>
       </c>
       <c r="B350" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C350" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E350" t="s">
         <v>1304</v>
-      </c>
-      <c r="E350" t="s">
-        <v>1305</v>
       </c>
       <c r="F350" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27800,13 +27800,13 @@
         <v>4</v>
       </c>
       <c r="B351" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C351" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E351" t="s">
         <v>1306</v>
-      </c>
-      <c r="E351" t="s">
-        <v>1307</v>
       </c>
       <c r="F351" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27831,13 +27831,13 @@
         <v>4</v>
       </c>
       <c r="B352" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C352" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E352" t="s">
         <v>1308</v>
-      </c>
-      <c r="E352" t="s">
-        <v>1309</v>
       </c>
       <c r="F352" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27862,13 +27862,13 @@
         <v>4</v>
       </c>
       <c r="B353" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C353" t="s">
         <v>541</v>
       </c>
       <c r="E353" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="F353" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27893,13 +27893,13 @@
         <v>4</v>
       </c>
       <c r="B354" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C354" t="s">
         <v>327</v>
       </c>
       <c r="E354" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="F354" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27924,13 +27924,13 @@
         <v>4</v>
       </c>
       <c r="B355" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C355" t="s">
         <v>1312</v>
       </c>
-      <c r="C355" t="s">
+      <c r="E355" t="s">
         <v>1313</v>
-      </c>
-      <c r="E355" t="s">
-        <v>1314</v>
       </c>
       <c r="F355" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27955,13 +27955,13 @@
         <v>4</v>
       </c>
       <c r="B356" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C356" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="E356" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="F356" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27986,13 +27986,13 @@
         <v>4</v>
       </c>
       <c r="B357" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C357" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="E357" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="F357" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28017,13 +28017,13 @@
         <v>4</v>
       </c>
       <c r="B358" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C358" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E358" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="F358" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28048,13 +28048,13 @@
         <v>4</v>
       </c>
       <c r="B359" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C359" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E359" t="s">
         <v>1326</v>
-      </c>
-      <c r="E359" t="s">
-        <v>1327</v>
       </c>
       <c r="F359" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28079,13 +28079,13 @@
         <v>4</v>
       </c>
       <c r="B360" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C360" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E360" t="s">
         <v>1328</v>
-      </c>
-      <c r="E360" t="s">
-        <v>1329</v>
       </c>
       <c r="F360" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28113,10 +28113,10 @@
         <v>890</v>
       </c>
       <c r="C361" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E361" t="s">
         <v>1331</v>
-      </c>
-      <c r="E361" t="s">
-        <v>1332</v>
       </c>
       <c r="F361" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28141,13 +28141,13 @@
         <v>4</v>
       </c>
       <c r="B362" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C362" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E362" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="F362" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28172,13 +28172,13 @@
         <v>4</v>
       </c>
       <c r="B363" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C363" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="E363" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="F363" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28203,13 +28203,13 @@
         <v>4</v>
       </c>
       <c r="B364" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C364" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E364" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="F364" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28234,13 +28234,13 @@
         <v>4</v>
       </c>
       <c r="B365" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C365" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E365" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="F365" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28265,13 +28265,13 @@
         <v>4</v>
       </c>
       <c r="B366" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C366" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="E366" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="F366" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28296,13 +28296,13 @@
         <v>4</v>
       </c>
       <c r="B367" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C367" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E367" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="F367" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28327,13 +28327,13 @@
         <v>4</v>
       </c>
       <c r="B368" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C368" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E368" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="F368" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28358,13 +28358,13 @@
         <v>4</v>
       </c>
       <c r="B369" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C369" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="E369" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="F369" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28389,13 +28389,13 @@
         <v>4</v>
       </c>
       <c r="B370" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C370" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E370" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="F370" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28420,13 +28420,13 @@
         <v>4</v>
       </c>
       <c r="B371" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C371" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="E371" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="F371" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28451,13 +28451,13 @@
         <v>4</v>
       </c>
       <c r="B372" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="C372" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E372" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="F372" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28485,10 +28485,10 @@
         <v>719</v>
       </c>
       <c r="C373" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E373" t="s">
         <v>1371</v>
-      </c>
-      <c r="E373" t="s">
-        <v>1372</v>
       </c>
       <c r="F373" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28516,10 +28516,10 @@
         <v>719</v>
       </c>
       <c r="C374" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E374" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="F374" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28547,10 +28547,10 @@
         <v>1062</v>
       </c>
       <c r="C375" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E375" t="s">
         <v>1386</v>
-      </c>
-      <c r="E375" t="s">
-        <v>1387</v>
       </c>
       <c r="F375" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28578,10 +28578,10 @@
         <v>724</v>
       </c>
       <c r="C376" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E376" t="s">
         <v>1411</v>
-      </c>
-      <c r="E376" t="s">
-        <v>1412</v>
       </c>
       <c r="F376" s="1" t="str">
         <f t="shared" si="40"/>
@@ -29323,7 +29323,7 @@
         <v>398</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -29821,7 +29821,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
@@ -29830,10 +29830,10 @@
         <v>200</v>
       </c>
       <c r="D41" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E41" t="s">
         <v>1238</v>
-      </c>
-      <c r="E41" t="s">
-        <v>1239</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -29863,7 +29863,7 @@
         <v>110</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -29881,7 +29881,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
@@ -29893,7 +29893,7 @@
         <v>304</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -29911,7 +29911,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -29923,7 +29923,7 @@
         <v>304</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Fixing missing Snugglepot dialogue
</commit_message>
<xml_diff>
--- a/mods/tuxemon/maps/Map Helper.xlsx
+++ b/mods/tuxemon/maps/Map Helper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\tuxemon-development-win64\exe.win-amd64-3.8\mods\tuxemon\maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\GitHub\Tuxemon\mods\tuxemon\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B3CCF4-85C6-4016-A9DC-ED0E73A7B168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D16AA4-5057-4FE1-B59D-6F880A4BC3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1412">
   <si>
     <t>Dante</t>
   </si>
@@ -4273,9 +4273,6 @@
   </si>
   <si>
     <t>Why yes, I am the inventor of the Extreme Restraints. \n What are they, I hear you ask? \n Only a set of manacles so powerful that even a dragon could not escape them. \n They are being used in the containment unit to make sure none of the infected tuxemon escape.</t>
-  </si>
-  <si>
-    <t>snugglepot2</t>
   </si>
   <si>
     <t>Wow! One day I'm going to be a trainer just like you!</t>
@@ -16461,8 +16458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB86BEE-659D-40E3-BE2C-991E3BDA8715}">
   <dimension ref="A1:R376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E286" sqref="E286"/>
+    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C377" sqref="C377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25766,7 +25763,7 @@
         <v>1122</v>
       </c>
       <c r="E285" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="F285" s="1" t="str">
         <f t="shared" si="40"/>
@@ -28578,26 +28575,26 @@
         <v>724</v>
       </c>
       <c r="C376" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E376" t="s">
         <v>1410</v>
-      </c>
-      <c r="E376" t="s">
-        <v>1411</v>
       </c>
       <c r="F376" s="1" t="str">
         <f t="shared" si="40"/>
-        <v>Talk snugglepot2</v>
+        <v>Talk snugglepot</v>
       </c>
       <c r="G376" t="str">
         <f t="shared" si="79"/>
-        <v>spyder_leatherhouse2_snugglepot2</v>
+        <v>spyder_leatherhouse2_snugglepot</v>
       </c>
       <c r="H376" t="str">
         <f t="shared" si="80"/>
-        <v>translated_dialog spyder_leatherhouse2_snugglepot2</v>
+        <v>translated_dialog spyder_leatherhouse2_snugglepot</v>
       </c>
       <c r="J376" t="str">
         <f t="shared" si="78"/>
-        <v xml:space="preserve">msgid "spyder_leatherhouse2_snugglepot2" 
+        <v xml:space="preserve">msgid "spyder_leatherhouse2_snugglepot" 
 msgstr "Wow! One day I'm going to be a trainer just like you!" </v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing Omnichannel HQ dialogue
Fixing missing dialogue spotted by ultidonki
</commit_message>
<xml_diff>
--- a/mods/tuxemon/maps/Map Helper.xlsx
+++ b/mods/tuxemon/maps/Map Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\GitHub\Tuxemon\mods\tuxemon\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D16AA4-5057-4FE1-B59D-6F880A4BC3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D4A495-4BC4-4ED6-82B9-A681C8CA0D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="1414">
   <si>
     <t>Dante</t>
   </si>
@@ -4279,6 +4279,12 @@
   </si>
   <si>
     <t>A newspaper clipping is on the wall. It begins: \n "The famous art critic has put away his poison pen and picked up the paint brush. \n After years of tearing down artists, can he do any better himself?"</t>
+  </si>
+  <si>
+    <t>Back again? I should have fed you into the meat grinder back at Scoop HQ.</t>
+  </si>
+  <si>
+    <t>You really are a diamond in the rough, aren't you?</t>
   </si>
 </sst>
 </file>
@@ -16458,8 +16464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB86BEE-659D-40E3-BE2C-991E3BDA8715}">
   <dimension ref="A1:R376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C377" sqref="C377"/>
+    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E346" sqref="E346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27653,6 +27659,9 @@
       <c r="C346" t="s">
         <v>461</v>
       </c>
+      <c r="E346" t="s">
+        <v>1413</v>
+      </c>
       <c r="F346" s="1" t="str">
         <f t="shared" si="40"/>
         <v>Talk zoolander1</v>
@@ -27668,7 +27677,7 @@
       <c r="J346" t="str">
         <f t="shared" si="68"/>
         <v xml:space="preserve">msgid "spyder_omnichannel_zoolander1" 
-msgstr "" </v>
+msgstr "You really are a diamond in the rough, aren't you?" </v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.3">
@@ -27680,6 +27689,9 @@
       </c>
       <c r="C347" t="s">
         <v>948</v>
+      </c>
+      <c r="E347" t="s">
+        <v>1412</v>
       </c>
       <c r="F347" s="1" t="str">
         <f t="shared" si="40"/>
@@ -27696,7 +27708,7 @@
       <c r="J347" t="str">
         <f t="shared" si="68"/>
         <v xml:space="preserve">msgid "spyder_omnichannel_donald1" 
-msgstr "" </v>
+msgstr "Back again? I should have fed you into the meat grinder back at Scoop HQ." </v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>